<commit_message>
blue marked cell, where to enter new entry, dark blue, where new data are required, light blue, where next entry can be entered
</commit_message>
<xml_diff>
--- a/Cash_Box.xlsx
+++ b/Cash_Box.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="24">
   <si>
     <t>Wasser, Toilettenpapier</t>
   </si>
@@ -66,12 +66,6 @@
     <t>Till Amount:</t>
   </si>
   <si>
-    <t>Kaffe</t>
-  </si>
-  <si>
-    <t>Notiz: diese Quittung muss noch ausbezahlt werden, weil der Kassenstand zu niedrig war.</t>
-  </si>
-  <si>
     <t>Name:</t>
   </si>
   <si>
@@ -84,16 +78,19 @@
     <t>drop-down select name:</t>
   </si>
   <si>
-    <t>employee 1</t>
+    <t>last filled row for insertation:</t>
   </si>
   <si>
-    <t>employee 2</t>
+    <t>Employee 1</t>
   </si>
   <si>
-    <t>employee 3</t>
+    <t>Employee 2</t>
   </si>
   <si>
-    <t>employee 4</t>
+    <t>Employee 3</t>
+  </si>
+  <si>
+    <t>Employee 4</t>
   </si>
 </sst>
 </file>
@@ -489,7 +486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -653,6 +650,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -684,7 +689,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
@@ -694,8 +699,15 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1017,10 +1029,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S80"/>
+  <dimension ref="A1:S77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:B20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,10 +1075,10 @@
         <v>8</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H2" s="16" t="s">
         <v>1</v>
@@ -1089,7 +1101,7 @@
         <v>50.01</v>
       </c>
       <c r="F3" s="49" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G3" s="38" t="s">
         <v>12</v>
@@ -1106,7 +1118,7 @@
         <v>-2.44</v>
       </c>
       <c r="D4" s="11">
-        <f t="shared" ref="D4:D34" si="0">IF(D3 = "",
+        <f t="shared" ref="D4:D21" si="0">IF(D3 = "",
     "",
     IF(D3 + C4 = D3,
         "",
@@ -1126,7 +1138,7 @@
         <v>47.57</v>
       </c>
       <c r="F4" s="42" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G4" s="39" t="s">
         <v>0</v>
@@ -1153,7 +1165,7 @@
         <v>50.01</v>
       </c>
       <c r="F5" s="49" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G5" s="40" t="s">
         <v>6</v>
@@ -1190,13 +1202,13 @@
         <v>44.43</v>
       </c>
       <c r="F6" s="42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G6" s="41" t="s">
         <v>4</v>
       </c>
       <c r="H6" s="51">
-        <f t="shared" ref="H6:H34" si="2">IF(OR(G6 = "Kassenausgleich", C6 = ""),
+        <f t="shared" ref="H6:H20" si="2">IF(OR(G6 = "Kassenausgleich", C6 = ""),
     "",
     IF(H5 &lt;&gt; "",
         H5 + 1,
@@ -1224,7 +1236,7 @@
         <v>37.35</v>
       </c>
       <c r="F7" s="42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G7" s="41" t="s">
         <v>2</v>
@@ -1252,7 +1264,7 @@
         <v>32.36</v>
       </c>
       <c r="F8" s="42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G8" s="41" t="s">
         <v>3</v>
@@ -1280,7 +1292,7 @@
         <v>27.369999999999997</v>
       </c>
       <c r="F9" s="42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G9" s="41" t="s">
         <v>3</v>
@@ -1308,7 +1320,7 @@
         <v>6.2499999999999964</v>
       </c>
       <c r="F10" s="42" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G10" s="41" t="s">
         <v>5</v>
@@ -1336,7 +1348,7 @@
         <v>2.5599999999999965</v>
       </c>
       <c r="F11" s="42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G11" s="41" t="s">
         <v>3</v>
@@ -1364,7 +1376,7 @@
         <v>48.76</v>
       </c>
       <c r="F12" s="49" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G12" s="40" t="s">
         <v>6</v>
@@ -1392,7 +1404,7 @@
         <v>46.989999999999995</v>
       </c>
       <c r="F13" s="42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G13" s="42" t="s">
         <v>2</v>
@@ -1420,7 +1432,7 @@
         <v>41.999999999999993</v>
       </c>
       <c r="F14" s="42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G14" s="42" t="s">
         <v>3</v>
@@ -1448,7 +1460,7 @@
         <v>37.009999999999991</v>
       </c>
       <c r="F15" s="42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G15" s="42" t="s">
         <v>3</v>
@@ -1476,7 +1488,7 @@
         <v>35.829999999999991</v>
       </c>
       <c r="F16" s="42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G16" s="42" t="s">
         <v>2</v>
@@ -1487,7 +1499,7 @@
       </c>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="35">
         <v>41562</v>
@@ -1504,7 +1516,7 @@
         <v>30.839999999999989</v>
       </c>
       <c r="F17" s="42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G17" s="42" t="s">
         <v>3</v>
@@ -1515,7 +1527,7 @@
       </c>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="35">
         <v>41570</v>
@@ -1532,7 +1544,7 @@
         <v>24.669999999999987</v>
       </c>
       <c r="F18" s="42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G18" s="42" t="s">
         <v>4</v>
@@ -1543,7 +1555,7 @@
       </c>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="35">
         <v>41576</v>
@@ -1560,10 +1572,10 @@
         <v>20.899999999999988</v>
       </c>
       <c r="F19" s="42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G19" s="43" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="H19" s="50">
         <f t="shared" si="2"/>
@@ -1571,7 +1583,7 @@
       </c>
       <c r="I19" s="4"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="35">
         <v>41578</v>
@@ -1594,7 +1606,7 @@
         <v>-5.5000000000000107</v>
       </c>
       <c r="F20" s="42" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G20" s="43" t="s">
         <v>5</v>
@@ -1604,31 +1616,36 @@
         <v>15</v>
       </c>
       <c r="I20" s="4"/>
-      <c r="J20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
-      <c r="B21" s="35"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="11" t="str">
+      <c r="B21" s="31">
+        <v>41584</v>
+      </c>
+      <c r="C21" s="56">
+        <v>55.5</v>
+      </c>
+      <c r="D21" s="12">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E21" s="11" t="str">
-        <f t="shared" ref="E21:E34" si="3">IF(E20 = "",
+        <v>-1.0000000000005116E-2</v>
+      </c>
+      <c r="E21" s="12">
+        <f t="shared" ref="E21" si="3">IF(E20 = "",
     "",
     IF(E20 + C21 = E20,
         "",
         E20 + C21
     )
 )</f>
-        <v/>
-      </c>
-      <c r="F21" s="42"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="50" t="str">
+        <v>49.999999999999986</v>
+      </c>
+      <c r="F21" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="53" t="str">
         <f>IF(OR(G21 = "Kassenausgleich", C21 = ""),
     "",
     IF(H20 &lt;&gt; "",
@@ -1640,349 +1657,368 @@
       </c>
       <c r="I21" s="4"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
-      <c r="B22" s="35"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E22" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="F22" s="42"/>
-      <c r="G22" s="43"/>
-      <c r="H22" s="50" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+      <c r="B22" s="35">
+        <v>41584</v>
+      </c>
+      <c r="C22" s="55">
+        <v>-4.99</v>
+      </c>
+      <c r="D22" s="10">
+        <f t="shared" ref="D22:D24" si="4">IF(D21 = "",
+    "",
+    IF(D21 + C22 = D21,
+        "",
+        D21 + C22
+    )
+)</f>
+        <v>-5.0000000000000053</v>
+      </c>
+      <c r="E22" s="10">
+        <f t="shared" ref="E22:E24" si="5">IF(E21 = "",
+    "",
+    IF(E21 + C22 = E21,
+        "",
+        E21 + C22
+    )
+)</f>
+        <v>45.009999999999984</v>
+      </c>
+      <c r="F22" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="H22" s="51">
+        <f t="shared" ref="H22:H24" si="6">IF(OR(G22 = "Kassenausgleich", C22 = ""),
+    "",
+    IF(H21 &lt;&gt; "",
+        H21 + 1,
+        H20 + 1
+    )
+)</f>
+        <v>16</v>
       </c>
       <c r="I22" s="4"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E23" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="F23" s="43"/>
-      <c r="G23" s="43"/>
-      <c r="H23" s="50" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+      <c r="B23" s="35">
+        <v>41584</v>
+      </c>
+      <c r="C23" s="37">
+        <v>-3.9</v>
+      </c>
+      <c r="D23" s="11">
+        <f t="shared" si="4"/>
+        <v>-8.9000000000000057</v>
+      </c>
+      <c r="E23" s="11">
+        <f t="shared" si="5"/>
+        <v>41.109999999999985</v>
+      </c>
+      <c r="F23" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="H23" s="50">
+        <f t="shared" si="6"/>
+        <v>17</v>
       </c>
       <c r="I23" s="4"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="35"/>
       <c r="C24" s="37"/>
       <c r="D24" s="11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="E24" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="F24" s="42"/>
       <c r="G24" s="43"/>
       <c r="H24" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I24" s="4"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="35"/>
       <c r="C25" s="37"/>
       <c r="D25" s="11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D25:D31" si="7">IF(D24 = "",
+    "",
+    IF(D24 + C25 = D24,
+        "",
+        D24 + C25
+    )
+)</f>
         <v/>
       </c>
       <c r="E25" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="E25:E31" si="8">IF(E24 = "",
+    "",
+    IF(E24 + C25 = E24,
+        "",
+        E24 + C25
+    )
+)</f>
         <v/>
       </c>
       <c r="F25" s="42"/>
       <c r="G25" s="43"/>
       <c r="H25" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="H25:H31" si="9">IF(OR(G25 = "Kassenausgleich", C25 = ""),
+    "",
+    IF(H24 &lt;&gt; "",
+        H24 + 1,
+        H23 + 1
+    )
+)</f>
         <v/>
       </c>
       <c r="I25" s="4"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="35"/>
       <c r="C26" s="37"/>
       <c r="D26" s="11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="E26" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="F26" s="42"/>
       <c r="G26" s="43"/>
       <c r="H26" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I26" s="4"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="35"/>
       <c r="C27" s="37"/>
       <c r="D27" s="11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="E27" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="F27" s="42"/>
       <c r="G27" s="43"/>
       <c r="H27" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I27" s="4"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="35"/>
       <c r="C28" s="37"/>
       <c r="D28" s="11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="E28" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="F28" s="42"/>
       <c r="G28" s="43"/>
       <c r="H28" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(OR(G28 = "Kassenausgleich", C28 = ""),
+    "",
+    IF(#REF! &lt;&gt; "",#REF! +
+ 1,#REF! +
+ 1
+    )
+)</f>
         <v/>
       </c>
       <c r="I28" s="4"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="35"/>
       <c r="C29" s="37"/>
       <c r="D29" s="11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="E29" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="F29" s="42"/>
       <c r="G29" s="43"/>
       <c r="H29" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(OR(G29 = "Kassenausgleich", C29 = ""),
+    "",
+    IF(H28 &lt;&gt; "",
+        H28 + 1,#REF! +
+ 1
+    )
+)</f>
         <v/>
       </c>
       <c r="I29" s="4"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="35"/>
       <c r="C30" s="37"/>
       <c r="D30" s="11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="E30" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="F30" s="42"/>
       <c r="G30" s="43"/>
       <c r="H30" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I30" s="4"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="35"/>
       <c r="C31" s="37"/>
       <c r="D31" s="11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="E31" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="F31" s="42"/>
       <c r="G31" s="43"/>
       <c r="H31" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I31" s="4"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
-      <c r="B32" s="35"/>
-      <c r="C32" s="37"/>
-      <c r="D32" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E32" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="F32" s="42"/>
-      <c r="G32" s="43"/>
-      <c r="H32" s="50" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
       <c r="I32" s="4"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
-      <c r="B33" s="35"/>
-      <c r="C33" s="37"/>
-      <c r="D33" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E33" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="F33" s="42"/>
-      <c r="G33" s="43"/>
-      <c r="H33" s="50" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="B33" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="22">
+        <f ca="1">SUM(C3:INDIRECT("C" &amp; Calculation!B3))</f>
+        <v>41.109999999999985</v>
+      </c>
+      <c r="D33" s="24">
+        <f ca="1">INDIRECT("D" &amp; Calculation!B3)</f>
+        <v>-8.9000000000000057</v>
+      </c>
+      <c r="E33" s="20">
+        <f ca="1">INDIRECT("E" &amp; Calculation!B3)</f>
+        <v>41.109999999999985</v>
+      </c>
+      <c r="F33" s="46"/>
+      <c r="G33" s="62"/>
+      <c r="H33" s="63"/>
       <c r="I33" s="4"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
-      <c r="B34" s="35"/>
-      <c r="C34" s="37"/>
-      <c r="D34" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E34" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="F34" s="42"/>
-      <c r="G34" s="43"/>
-      <c r="H34" s="50" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="B34" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="19">
+        <f>$C$3</f>
+        <v>50.01</v>
+      </c>
+      <c r="D34" s="60">
+        <f ca="1">E33 - D33</f>
+        <v>50.009999999999991</v>
+      </c>
+      <c r="E34" s="61"/>
+      <c r="F34" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" s="64"/>
+      <c r="H34" s="65"/>
       <c r="I34" s="4"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
       <c r="I35" s="4"/>
     </row>
-    <row r="36" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="4"/>
-      <c r="B36" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="C36" s="22">
-        <f ca="1">SUM(C3:INDIRECT("C" &amp; Calculation!B3))</f>
-        <v>-5.5000000000000107</v>
-      </c>
-      <c r="D36" s="24">
-        <f ca="1">INDIRECT("D" &amp; Calculation!B3)</f>
-        <v>-55.510000000000005</v>
-      </c>
-      <c r="E36" s="20">
-        <f ca="1">INDIRECT("E" &amp; Calculation!B3)</f>
-        <v>-5.5000000000000107</v>
-      </c>
-      <c r="F36" s="46"/>
-      <c r="G36" s="60"/>
-      <c r="H36" s="61"/>
-      <c r="I36" s="4"/>
-    </row>
-    <row r="37" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-      <c r="B37" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C37" s="19">
-        <f>$C$3</f>
-        <v>50.01</v>
-      </c>
-      <c r="D37" s="58">
-        <f ca="1">E36 - D36</f>
-        <v>50.009999999999991</v>
-      </c>
-      <c r="E37" s="59"/>
-      <c r="F37" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="G37" s="62"/>
-      <c r="H37" s="63"/>
-      <c r="I37" s="4"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="4"/>
-    </row>
-    <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E39"/>
-    </row>
-    <row r="40" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C40" s="55" t="str">
-        <f ca="1">IF( AND(C37 = D37, AND( C36-D36 = C37, C36 = E36 )),
+    <row r="36" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E36"/>
+    </row>
+    <row r="37" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C37" s="57" t="str">
+        <f ca="1">IF( AND(C34 = D34, AND( C33-D33 = C34, C33 = E33 )),
 "Calculations successfully finished!",
 "Error, calculations are incorrect!"
 )</f>
         <v>Calculations successfully finished!</v>
       </c>
-      <c r="D40" s="56"/>
-      <c r="E40" s="57"/>
-    </row>
-    <row r="41" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="D37" s="58"/>
+      <c r="E37" s="59"/>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E39" s="7"/>
+      <c r="F39" s="25"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B40"/>
+      <c r="C40"/>
+      <c r="D40"/>
+      <c r="E40"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B41"/>
+      <c r="C41" s="13"/>
+      <c r="D41"/>
+      <c r="E41" s="13"/>
+    </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E42" s="7"/>
-      <c r="F42" s="25"/>
+      <c r="E42"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B43"/>
@@ -1992,11 +2028,14 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B44"/>
-      <c r="C44" s="13"/>
+      <c r="C44"/>
       <c r="D44"/>
-      <c r="E44" s="13"/>
+      <c r="E44"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B45"/>
+      <c r="C45"/>
+      <c r="D45"/>
       <c r="E45"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -2190,24 +2229,6 @@
       <c r="C77"/>
       <c r="D77"/>
       <c r="E77"/>
-    </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B78"/>
-      <c r="C78"/>
-      <c r="D78"/>
-      <c r="E78"/>
-    </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B79"/>
-      <c r="C79"/>
-      <c r="D79"/>
-      <c r="E79"/>
-    </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B80"/>
-      <c r="C80"/>
-      <c r="D80"/>
-      <c r="E80"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
@@ -2215,56 +2236,44 @@
     <sortCondition ref="L3"/>
   </sortState>
   <mergeCells count="3">
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="G36:H37"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="G33:H34"/>
   </mergeCells>
-  <conditionalFormatting sqref="C40">
-    <cfRule type="containsText" dxfId="4" priority="41" operator="containsText" text="incorrect">
-      <formula>NOT(ISERROR(SEARCH("incorrect",C40)))</formula>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="5" priority="45" operator="containsText" text="incorrect">
+      <formula>NOT(ISERROR(SEARCH("incorrect",C37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="42" operator="containsText" text="successfull">
-      <formula>NOT(ISERROR(SEARCH("successfull",C40)))</formula>
+    <cfRule type="containsText" dxfId="4" priority="47" operator="containsText" text="successfull">
+      <formula>NOT(ISERROR(SEARCH("successfull",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:H34">
-    <cfRule type="expression" dxfId="2" priority="40">
+  <conditionalFormatting sqref="B2:H31">
+    <cfRule type="expression" dxfId="3" priority="44">
       <formula>ROW()=EVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:H34">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>(INDIRECT("C" &amp; ROW() - 1) = "")</formula>
+  <conditionalFormatting sqref="B3:C31 F3:G31">
+    <cfRule type="expression" dxfId="2" priority="43">
+      <formula>AND(ROW()&gt;=INDIRECT("Calculation!F"&amp;3)+1,ROW()&lt;=INDIRECT("Calculation!B"&amp;3)+1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>ROW()=INDIRECT("Calculation!B"&amp;3)+1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>AND(INDIRECT("Calculation!B"&amp;3)=INDIRECT("Calculation!F"&amp;3),ROW()=INDIRECT("Calculation!B"&amp;3)+1)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="notContainsText" priority="34" operator="notContains" id="{0935EA63-FB09-44DA-8A67-823740E0701D}">
-            <xm:f>ISERROR(SEARCH("",B3))</xm:f>
-            <xm:f>""</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="3" tint="0.39994506668294322"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>B3:C34 F3:G34</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Calculation!$D$3:$D$7</xm:f>
           </x14:formula1>
-          <xm:sqref>F3:F34</xm:sqref>
+          <xm:sqref>F3:F31</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2277,16 +2286,18 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2.85546875" customWidth="1"/>
     <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2.85546875" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -2295,57 +2306,75 @@
       <c r="C1" s="44"/>
       <c r="D1" s="44"/>
       <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="44"/>
       <c r="B2" s="45" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C2" s="44"/>
       <c r="D2" s="47" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E2" s="44"/>
+      <c r="F2" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="44"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="44"/>
       <c r="B3" s="45">
-        <f t="array" ref="B3">ROW(INDEX(Cash_Box!C:C, MAX((Cash_Box!C3:C34 &lt;&gt; "") * (ROW(Cash_Box!C3:C34)))))</f>
-        <v>20</v>
+        <f t="array" ref="B3">ROW(INDEX(Cash_Box!C:C, MAX((Cash_Box!C3:C31 &lt;&gt; "") * (ROW(Cash_Box!C3:C31)))))</f>
+        <v>23</v>
       </c>
       <c r="C3" s="44"/>
       <c r="D3" s="48"/>
       <c r="E3" s="44"/>
+      <c r="F3" s="45">
+        <f t="array" ref="F3">MIN(
+    ROW(INDEX(Cash_Box!B:B, MAX((Cash_Box!B3:B31 &lt;&gt; "") * (ROW(Cash_Box!B3:B31))))),
+    ROW(INDEX(Cash_Box!C:C, MAX((Cash_Box!C3:C31 &lt;&gt; "") * (ROW(Cash_Box!C3:C31))))),
+    ROW(INDEX(Cash_Box!F:F, MAX((Cash_Box!F3:F31 &lt;&gt; "") * (ROW(Cash_Box!F3:F31))))),
+    ROW(INDEX(Cash_Box!G:G, MAX((Cash_Box!G3:G31 &lt;&gt; "") * (ROW(Cash_Box!G3:G31)))))
+)</f>
+        <v>23</v>
+      </c>
+      <c r="G3" s="44"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="44"/>
       <c r="B4" s="44"/>
       <c r="C4" s="44"/>
       <c r="D4" s="48" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="44"/>
       <c r="D5" s="48" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="44"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C6" s="44"/>
       <c r="D6" s="48" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" s="44"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C7" s="44"/>
       <c r="D7" s="48" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" s="44"/>
     </row>

</xml_diff>